<commit_message>
Some more flask so I can pull from a nano
</commit_message>
<xml_diff>
--- a/pi_breakout/Project Outputs for pi_breakout/pi_breakout.xlsx
+++ b/pi_breakout/Project Outputs for pi_breakout/pi_breakout.xlsx
@@ -1,11 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FDAC114E-A705-48F6-91D6-7DB0AF99C3AD}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ben\Documents\Projects\Projects\pi_breakout\Project Outputs for pi_breakout\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BBBF998-222B-4262-8746-8425CED3F463}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2835" yWindow="2055" windowWidth="15345" windowHeight="11385" xr2:uid="{E0233625-D3CE-4CF5-87FA-1C41BDF76AA0}"/>
+    <workbookView xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="11385" xr2:uid="{1D14A2ED-0A3D-4E24-B993-2ACD3398E1EA}"/>
   </bookViews>
   <sheets>
     <sheet name="pi_breakout" sheetId="1" r:id="rId1"/>
@@ -26,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="240">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="240">
   <si>
     <t>Comment</t>
   </si>
@@ -767,7 +772,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -777,6 +782,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor indexed="22"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -808,13 +819,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1128,10 +1140,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6A98D6F-0665-41AF-AFF8-112B5EA39116}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC0DE2DB-7B9E-4608-B5DE-D955999BD958}">
   <dimension ref="A1:M30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="E30" sqref="D30:E30"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1189,10 +1203,10 @@
       <c r="C2" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="4" t="s">
         <v>17</v>
       </c>
       <c r="F2" s="2" t="s">
@@ -1230,10 +1244,10 @@
       <c r="C3" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E3" s="4" t="s">
         <v>29</v>
       </c>
       <c r="F3" s="2" t="s">
@@ -1271,10 +1285,10 @@
       <c r="C4" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="E4" s="4" t="s">
         <v>40</v>
       </c>
       <c r="F4" s="2" t="s">
@@ -1312,10 +1326,10 @@
       <c r="C5" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="E5" s="4" t="s">
         <v>50</v>
       </c>
       <c r="F5" s="2" t="s">
@@ -1353,10 +1367,10 @@
       <c r="C6" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D6" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="E6" s="4" t="s">
         <v>59</v>
       </c>
       <c r="F6" s="2" t="s">
@@ -1394,10 +1408,10 @@
       <c r="C7" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D7" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="E7" s="2" t="s">
+      <c r="E7" s="4" t="s">
         <v>67</v>
       </c>
       <c r="F7" s="2" t="s">
@@ -1435,10 +1449,10 @@
       <c r="C8" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D8" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="E8" s="4" t="s">
         <v>75</v>
       </c>
       <c r="F8" s="2" t="s">
@@ -1476,10 +1490,10 @@
       <c r="C9" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="D9" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="E9" s="2" t="s">
+      <c r="E9" s="4" t="s">
         <v>83</v>
       </c>
       <c r="F9" s="2" t="s">
@@ -1517,10 +1531,10 @@
       <c r="C10" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="D10" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="E10" s="2" t="s">
+      <c r="E10" s="4" t="s">
         <v>94</v>
       </c>
       <c r="F10" s="2" t="s">
@@ -1558,10 +1572,10 @@
       <c r="C11" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="D11" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="E11" s="2" t="s">
+      <c r="E11" s="4" t="s">
         <v>104</v>
       </c>
       <c r="F11" s="2" t="s">
@@ -1599,10 +1613,10 @@
       <c r="C12" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="D12" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="E12" s="2" t="s">
+      <c r="E12" s="4" t="s">
         <v>113</v>
       </c>
       <c r="F12" s="2" t="s">
@@ -1927,10 +1941,10 @@
       <c r="C20" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="D20" s="2" t="s">
+      <c r="D20" s="4" t="s">
         <v>150</v>
       </c>
-      <c r="E20" s="2" t="s">
+      <c r="E20" s="4" t="s">
         <v>151</v>
       </c>
       <c r="F20" s="2" t="s">
@@ -1968,10 +1982,10 @@
       <c r="C21" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="D21" s="2" t="s">
+      <c r="D21" s="4" t="s">
         <v>161</v>
       </c>
-      <c r="E21" s="2" t="s">
+      <c r="E21" s="4" t="s">
         <v>162</v>
       </c>
       <c r="F21" s="2" t="s">
@@ -2009,10 +2023,10 @@
       <c r="C22" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="D22" s="2" t="s">
+      <c r="D22" s="4" t="s">
         <v>170</v>
       </c>
-      <c r="E22" s="2" t="s">
+      <c r="E22" s="4" t="s">
         <v>171</v>
       </c>
       <c r="F22" s="2" t="s">
@@ -2050,10 +2064,10 @@
       <c r="C23" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="D23" s="2" t="s">
+      <c r="D23" s="4" t="s">
         <v>177</v>
       </c>
-      <c r="E23" s="2" t="s">
+      <c r="E23" s="4" t="s">
         <v>178</v>
       </c>
       <c r="F23" s="2" t="s">
@@ -2091,10 +2105,10 @@
       <c r="C24" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="D24" s="2" t="s">
+      <c r="D24" s="4" t="s">
         <v>184</v>
       </c>
-      <c r="E24" s="2" t="s">
+      <c r="E24" s="4" t="s">
         <v>185</v>
       </c>
       <c r="F24" s="2" t="s">
@@ -2132,10 +2146,10 @@
       <c r="C25" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="D25" s="2" t="s">
+      <c r="D25" s="4" t="s">
         <v>191</v>
       </c>
-      <c r="E25" s="2" t="s">
+      <c r="E25" s="4" t="s">
         <v>192</v>
       </c>
       <c r="F25" s="2" t="s">
@@ -2173,10 +2187,10 @@
       <c r="C26" s="2" t="s">
         <v>199</v>
       </c>
-      <c r="D26" s="2" t="s">
+      <c r="D26" s="4" t="s">
         <v>200</v>
       </c>
-      <c r="E26" s="2" t="s">
+      <c r="E26" s="4" t="s">
         <v>201</v>
       </c>
       <c r="F26" s="2" t="s">
@@ -2214,10 +2228,10 @@
       <c r="C27" s="2" t="s">
         <v>206</v>
       </c>
-      <c r="D27" s="2" t="s">
+      <c r="D27" s="4" t="s">
         <v>207</v>
       </c>
-      <c r="E27" s="2" t="s">
+      <c r="E27" s="4" t="s">
         <v>208</v>
       </c>
       <c r="F27" s="2" t="s">
@@ -2255,10 +2269,10 @@
       <c r="C28" s="2" t="s">
         <v>214</v>
       </c>
-      <c r="D28" s="2" t="s">
+      <c r="D28" s="4" t="s">
         <v>215</v>
       </c>
-      <c r="E28" s="2" t="s">
+      <c r="E28" s="4" t="s">
         <v>216</v>
       </c>
       <c r="F28" s="2" t="s">
@@ -2296,10 +2310,10 @@
       <c r="C29" s="2" t="s">
         <v>222</v>
       </c>
-      <c r="D29" s="2" t="s">
+      <c r="D29" s="4" t="s">
         <v>223</v>
       </c>
-      <c r="E29" s="2" t="s">
+      <c r="E29" s="4" t="s">
         <v>224</v>
       </c>
       <c r="F29" s="2" t="s">
@@ -2337,10 +2351,10 @@
       <c r="C30" s="2" t="s">
         <v>231</v>
       </c>
-      <c r="D30" s="2" t="s">
+      <c r="D30" s="4" t="s">
         <v>232</v>
       </c>
-      <c r="E30" s="2" t="s">
+      <c r="E30" s="4" t="s">
         <v>233</v>
       </c>
       <c r="F30" s="2" t="s">

</xml_diff>